<commit_message>
Update excel export code
</commit_message>
<xml_diff>
--- a/wallet_tracker.xlsx
+++ b/wallet_tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Wallet Address</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Day 10 Night</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Total Night</t>
   </si>
   <si>
     <t>addr1qyfc2s7vk4cpua5cga9r8t5e69dc6nutp44snaq2tc7lq9kp8gyrycvlahf2h9gn6sdqxvpvrup2vtd2ewpp0e6thmlqmpnurs</t>
@@ -88,7 +88,7 @@
     <t>addr1qx3wf9xqlq9lp59ygujfp2z5ky2u4cv4edtf7dyjnhjve50nzf6stcvj4jauyjlwxsedlvmq9mvc9ucj9wc705ukksasjdssa2</t>
   </si>
   <si>
-    <t>Total All</t>
+    <t>Total Solution</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -445,13 +445,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2">
         <v>388.29</v>
       </c>
       <c r="D2">
-        <v>569.29</v>
+        <v>388.29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -459,13 +459,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C3">
         <v>392.0411</v>
       </c>
       <c r="D3">
-        <v>573.0410999999999</v>
+        <v>392.0411</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -473,13 +473,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C4">
         <v>385.2151</v>
       </c>
       <c r="D4">
-        <v>564.2151</v>
+        <v>385.2151</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -487,13 +487,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C5">
         <v>384.4421</v>
       </c>
       <c r="D5">
-        <v>565.4421</v>
+        <v>384.4421</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -501,13 +501,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C6">
         <v>390.0327</v>
       </c>
       <c r="D6">
-        <v>574.0327</v>
+        <v>390.0327</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -515,13 +515,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C7">
         <v>383.1463</v>
       </c>
       <c r="D7">
-        <v>563.1463</v>
+        <v>383.1463</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -529,13 +529,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C8">
         <v>388.8807</v>
       </c>
       <c r="D8">
-        <v>570.8806999999999</v>
+        <v>388.8807</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -549,7 +549,7 @@
         <v>401.2084</v>
       </c>
       <c r="D9">
-        <v>585.2084</v>
+        <v>401.2084</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -563,7 +563,7 @@
         <v>7.0614</v>
       </c>
       <c r="D10">
-        <v>18.0614</v>
+        <v>7.0614</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -577,7 +577,7 @@
         <v>7.0614</v>
       </c>
       <c r="D11">
-        <v>18.0614</v>
+        <v>7.0614</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -591,7 +591,7 @@
         <v>7.0614</v>
       </c>
       <c r="D12">
-        <v>18.0614</v>
+        <v>7.0614</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -605,7 +605,7 @@
         <v>7.0614</v>
       </c>
       <c r="D13">
-        <v>18.0614</v>
+        <v>7.0614</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -619,7 +619,7 @@
         <v>7.0614</v>
       </c>
       <c r="D14">
-        <v>18.0614</v>
+        <v>7.0614</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -633,7 +633,7 @@
         <v>7.0614</v>
       </c>
       <c r="D15">
-        <v>18.0614</v>
+        <v>7.0614</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -647,7 +647,7 @@
         <v>5.6491</v>
       </c>
       <c r="D16">
-        <v>15.6491</v>
+        <v>5.6491</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -661,7 +661,7 @@
         <v>5.6491</v>
       </c>
       <c r="D17">
-        <v>15.6491</v>
+        <v>5.6491</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -675,7 +675,7 @@
         <v>5.6491</v>
       </c>
       <c r="D18">
-        <v>15.6491</v>
+        <v>5.6491</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -689,7 +689,7 @@
         <v>409.8895</v>
       </c>
       <c r="D19">
-        <v>597.8895</v>
+        <v>409.8895</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -703,7 +703,7 @@
         <v>5.6491</v>
       </c>
       <c r="D20">
-        <v>15.6491</v>
+        <v>5.6491</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -711,13 +711,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>5.6491</v>
       </c>
       <c r="D21">
-        <v>14.6491</v>
+        <v>5.6491</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -725,13 +725,27 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>1755</v>
+        <v>1763</v>
       </c>
       <c r="C22">
         <v>3593.7598000000007</v>
       </c>
       <c r="D22">
-        <v>5348.759800000001</v>
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>1763</v>
+      </c>
+      <c r="C23">
+        <v>3593.7598000000007</v>
+      </c>
+      <c r="D23">
+        <v>3593.7598000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>